<commit_message>
IN-951 Add DB validations for ledger entries and ledger entry allocations
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Ledger.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Ledger.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5149841D-F1C4-684A-953B-6C7EDD31D3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0182CD-488E-1046-80DF-8AA6F949085D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31980" yWindow="5160" windowWidth="31740" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="3760" windowWidth="31740" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="78">
   <si>
     <t>table_name</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Populated via post-migration task</t>
   </si>
   <si>
-    <t>Linked to existing Finance Person via post-migration task</t>
-  </si>
-  <si>
     <t>finance_ledger</t>
   </si>
   <si>
@@ -224,12 +221,6 @@
     <t>credit_type_from_invoice_ref</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Probably not used but TBC with Elizabeth</t>
-  </si>
-  <si>
     <t>Should be left blank</t>
   </si>
   <si>
@@ -258,6 +249,12 @@
   </si>
   <si>
     <t>APPROVED</t>
+  </si>
+  <si>
+    <t>Linked to existing Finance Person via business rule</t>
+  </si>
+  <si>
+    <t>Should be left blank. Aged Debt will confirm the ledger entry</t>
   </si>
 </sst>
 </file>
@@ -639,16 +636,16 @@
     </row>
     <row r="2" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>30</v>
@@ -657,10 +654,10 @@
         <v>40</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
@@ -687,7 +684,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -761,10 +758,10 @@
     </row>
     <row r="2" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>16</v>
@@ -776,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -789,10 +786,10 @@
     </row>
     <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>33</v>
@@ -807,27 +804,27 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>44</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="5" t="b">
         <v>0</v>
@@ -847,13 +844,13 @@
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>21</v>
@@ -865,7 +862,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="M5" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O5" s="8" t="s">
         <v>18</v>
@@ -873,16 +870,16 @@
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="5" t="b">
         <v>0</v>
@@ -896,7 +893,7 @@
         <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>18</v>
@@ -904,13 +901,13 @@
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>21</v>
@@ -922,7 +919,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="M7" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>18</v>
@@ -930,13 +927,13 @@
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>21</v>
@@ -953,7 +950,7 @@
         <v>41</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>18</v>
@@ -961,13 +958,13 @@
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>21</v>
@@ -979,19 +976,19 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="M9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>31</v>
@@ -1011,18 +1008,18 @@
         <v>18</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>17</v>
@@ -1034,18 +1031,16 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="O11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>68</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>35</v>
@@ -1062,7 +1057,7 @@
       </c>
       <c r="H12" s="5"/>
       <c r="O12" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>46</v>
@@ -1070,10 +1065,10 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>37</v>
@@ -1088,19 +1083,21 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="O13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="P13" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>20</v>
@@ -1123,10 +1120,10 @@
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>38</v>
@@ -1149,16 +1146,16 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="E16" s="5" t="b">
         <v>0</v>
@@ -1170,18 +1167,18 @@
         <v>44</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>21</v>
@@ -1196,15 +1193,15 @@
         <v>44</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
IN-951 Add DB validations for ledger entries and ledger entry allocations (#462)
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Ledger.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Ledger.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5149841D-F1C4-684A-953B-6C7EDD31D3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0182CD-488E-1046-80DF-8AA6F949085D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31980" yWindow="5160" windowWidth="31740" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="3760" windowWidth="31740" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="78">
   <si>
     <t>table_name</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Populated via post-migration task</t>
   </si>
   <si>
-    <t>Linked to existing Finance Person via post-migration task</t>
-  </si>
-  <si>
     <t>finance_ledger</t>
   </si>
   <si>
@@ -224,12 +221,6 @@
     <t>credit_type_from_invoice_ref</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Probably not used but TBC with Elizabeth</t>
-  </si>
-  <si>
     <t>Should be left blank</t>
   </si>
   <si>
@@ -258,6 +249,12 @@
   </si>
   <si>
     <t>APPROVED</t>
+  </si>
+  <si>
+    <t>Linked to existing Finance Person via business rule</t>
+  </si>
+  <si>
+    <t>Should be left blank. Aged Debt will confirm the ledger entry</t>
   </si>
 </sst>
 </file>
@@ -639,16 +636,16 @@
     </row>
     <row r="2" spans="1:8" s="5" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>30</v>
@@ -657,10 +654,10 @@
         <v>40</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
@@ -687,7 +684,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -761,10 +758,10 @@
     </row>
     <row r="2" spans="1:16" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>16</v>
@@ -776,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -789,10 +786,10 @@
     </row>
     <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>33</v>
@@ -807,27 +804,27 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O3" s="10" t="s">
         <v>44</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="5" t="b">
         <v>0</v>
@@ -847,13 +844,13 @@
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>21</v>
@@ -865,7 +862,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="M5" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O5" s="8" t="s">
         <v>18</v>
@@ -873,16 +870,16 @@
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="5" t="b">
         <v>0</v>
@@ -896,7 +893,7 @@
         <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>18</v>
@@ -904,13 +901,13 @@
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>21</v>
@@ -922,7 +919,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="M7" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>18</v>
@@ -930,13 +927,13 @@
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>21</v>
@@ -953,7 +950,7 @@
         <v>41</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>18</v>
@@ -961,13 +958,13 @@
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>21</v>
@@ -979,19 +976,19 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="M9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>31</v>
@@ -1011,18 +1008,18 @@
         <v>18</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>17</v>
@@ -1034,18 +1031,16 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="O11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>68</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>35</v>
@@ -1062,7 +1057,7 @@
       </c>
       <c r="H12" s="5"/>
       <c r="O12" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>46</v>
@@ -1070,10 +1065,10 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>37</v>
@@ -1088,19 +1083,21 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="O13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="P13" s="8"/>
+        <v>18</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>20</v>
@@ -1123,10 +1120,10 @@
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>38</v>
@@ -1149,16 +1146,16 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="E16" s="5" t="b">
         <v>0</v>
@@ -1170,18 +1167,18 @@
         <v>44</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>21</v>
@@ -1196,15 +1193,15 @@
         <v>44</v>
       </c>
       <c r="P17" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Fix other erroneous mappings
* Some of the warnings tables had is_complete=Yes. This means they
  were previously excluded from validation. When I made the change
  to recognise these fields as being complete and mapped, the
  validation SQL failed, as the casrec_table was set for these
  fields in the spreadsheet, but casrec_column_name was not. By
  removing values from both of these columns in the spreadsheet,
  the default is used to construct the validation SQL.
* The finance_ledger spreadsheet had is_complete=YES for the reference
  field. This was not correctly treated as is_complete=yes, so the
  field was being ignored in the validation SQL. Once this changed so
  that it was included, the validation failed, as the reference
  field is populated with a UUID. By ignoring this during validation,
  we are still able to auto-generate the validation SQL for this table.
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Ledger.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Ledger.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F87305-1697-C74E-8EF6-E1E2C2317892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C575900A-6D35-8D42-A567-EFEC6EBF5184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="500" windowWidth="31740" windowHeight="19900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="500" windowWidth="38240" windowHeight="19900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>

</xml_diff>